<commit_message>
added exercise stats, update getExercise
</commit_message>
<xml_diff>
--- a/pipeline/Machine Learning.xlsx
+++ b/pipeline/Machine Learning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivany\fitai\pipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC62767B-BCA4-4DE1-9E68-815CE62B9893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B43AA48-9DD4-4DD0-BEDB-545025161EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1095" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="16">
   <si>
     <t>Rep No</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>New 2</t>
+  </si>
+  <si>
+    <t>Hamstring Stretch (Left Leg)</t>
+  </si>
+  <si>
+    <t>New 1</t>
   </si>
 </sst>
 </file>
@@ -409,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA64"/>
+  <dimension ref="A1:AK64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="AB7" sqref="AB7"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,7 +437,7 @@
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -441,8 +447,11 @@
       <c r="T1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,8 +524,35 @@
       <c r="Z2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -595,8 +631,37 @@
         <f>Y3-$Y$12</f>
         <v>2.4742179446749876E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>0.72158106656586096</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>51</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>37</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>1.28055810928344E-2</v>
+      </c>
+      <c r="AI3" s="1">
+        <v>-7.5664520263671797E-3</v>
+      </c>
+      <c r="AJ3" s="1">
+        <f>AH3-$AH$12</f>
+        <v>6.4915776252746415E-2</v>
+      </c>
+      <c r="AK3" s="1">
+        <f>AI3-$AI$12</f>
+        <v>-8.3268827862209502E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -675,8 +740,37 @@
         <f t="shared" ref="AA4:AA11" si="1">Y4-$Y$12</f>
         <v>3.4784131579928865E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>0.69077662240920601</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>37</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>34</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>-9.6017122268676702E-2</v>
+      </c>
+      <c r="AI4" s="1">
+        <v>3.5555601119995103E-2</v>
+      </c>
+      <c r="AJ4" s="1">
+        <f t="shared" ref="AJ4:AJ11" si="2">AH4-$AH$12</f>
+        <v>-4.390692710876469E-2</v>
+      </c>
+      <c r="AK4" s="1">
+        <f t="shared" ref="AK4:AK11" si="3">AI4-$AI$12</f>
+        <v>-4.0146774715847225E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -755,8 +849,37 @@
         <f t="shared" si="1"/>
         <v>7.4098640018038647E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>0.72268921439524503</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>5</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>39</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>1.5538096427917401E-2</v>
+      </c>
+      <c r="AI5" s="1">
+        <v>3.4094929695129297E-2</v>
+      </c>
+      <c r="AJ5" s="1">
+        <f t="shared" si="2"/>
+        <v>6.7648291587829409E-2</v>
+      </c>
+      <c r="AK5" s="1">
+        <f t="shared" si="3"/>
+        <v>-4.1607446140713031E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -835,8 +958,37 @@
         <f t="shared" si="1"/>
         <v>-2.9815978474086721E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC6" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>0.72070594207213901</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>20</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>34</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>-5.64336776733398E-3</v>
+      </c>
+      <c r="AI6" s="1">
+        <v>5.8874189853668199E-2</v>
+      </c>
+      <c r="AJ6" s="1">
+        <f t="shared" si="2"/>
+        <v>4.6466827392578035E-2</v>
+      </c>
+      <c r="AK6" s="1">
+        <f t="shared" si="3"/>
+        <v>-1.6828185982174129E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -915,8 +1067,37 @@
         <f t="shared" si="1"/>
         <v>-2.4508184856838228E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC7" s="1">
+        <v>5</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>0.72119018361228904</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>23</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>21</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>2.7883291244506801E-2</v>
+      </c>
+      <c r="AI7" s="1">
+        <v>2.94324159622192E-2</v>
+      </c>
+      <c r="AJ7" s="1">
+        <f t="shared" si="2"/>
+        <v>7.9993486404418807E-2</v>
+      </c>
+      <c r="AK7" s="1">
+        <f t="shared" si="3"/>
+        <v>-4.6269959873623132E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -995,8 +1176,37 @@
         <f t="shared" si="1"/>
         <v>1.2245350413851872E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>0.70638232408676505</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>29</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>35</v>
+      </c>
+      <c r="AG8" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>-4.84662055969238E-2</v>
+      </c>
+      <c r="AI8" s="1">
+        <v>8.2111299037933294E-2</v>
+      </c>
+      <c r="AJ8" s="1">
+        <f t="shared" si="2"/>
+        <v>3.6439895629882119E-3</v>
+      </c>
+      <c r="AK8" s="1">
+        <f t="shared" si="3"/>
+        <v>6.4089232020909659E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -1075,8 +1285,37 @@
         <f t="shared" si="1"/>
         <v>1.3407640986971878E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC9" s="1">
+        <v>2</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>0.70846825796900403</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>9</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>59</v>
+      </c>
+      <c r="AG9" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH9" s="1">
+        <v>-5.1817178726196199E-2</v>
+      </c>
+      <c r="AI9" s="1">
+        <v>0.109801232814788</v>
+      </c>
+      <c r="AJ9" s="1">
+        <f t="shared" si="2"/>
+        <v>2.9301643371581337E-4</v>
+      </c>
+      <c r="AK9" s="1">
+        <f t="shared" si="3"/>
+        <v>3.4098856978945671E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -1155,8 +1394,37 @@
         <f t="shared" si="1"/>
         <v>1.6812735133700865E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC10" s="1">
+        <v>3</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>0.69042242010880805</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>8</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>52</v>
+      </c>
+      <c r="AG10" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH10" s="1">
+        <v>-0.11832201480865399</v>
+      </c>
+      <c r="AI10" s="1">
+        <v>0.14246112108230499</v>
+      </c>
+      <c r="AJ10" s="1">
+        <f t="shared" si="2"/>
+        <v>-6.6211819648741982E-2</v>
+      </c>
+      <c r="AK10" s="1">
+        <f t="shared" si="3"/>
+        <v>6.6758745246462664E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -1235,8 +1503,37 @@
         <f t="shared" si="1"/>
         <v>-5.5077738232082327E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AC11" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>0.67636366173634999</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>42</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>23</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH11" s="1">
+        <v>-0.20495283603668199</v>
+      </c>
+      <c r="AI11" s="1">
+        <v>0.19655704498290999</v>
+      </c>
+      <c r="AJ11" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.15284264087676996</v>
+      </c>
+      <c r="AK11" s="1">
+        <f t="shared" si="3"/>
+        <v>0.12085466914706766</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -1295,31 +1592,63 @@
         <v>0.51726334533521978</v>
       </c>
       <c r="V12" s="1">
-        <f t="shared" ref="V12:AA12" si="2">AVERAGE(V3:V11)</f>
+        <f t="shared" ref="V12:AA12" si="4">AVERAGE(V3:V11)</f>
         <v>12.555555555555555</v>
       </c>
       <c r="W12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.666666666666667</v>
       </c>
       <c r="X12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9.3333333333333339</v>
       </c>
       <c r="Y12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.11861485905117412</v>
       </c>
       <c r="Z12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-5.0355672836303662E-2</v>
       </c>
       <c r="AA12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-6.1679056923619804E-18</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AD12" s="1">
+        <f>AVERAGE(AD3:AD11)</f>
+        <v>0.70650885477285186</v>
+      </c>
+      <c r="AE12" s="1">
+        <f t="shared" ref="AE12:AK12" si="5">AVERAGE(AE3:AE11)</f>
+        <v>24.888888888888889</v>
+      </c>
+      <c r="AF12" s="1">
+        <f t="shared" si="5"/>
+        <v>37.111111111111114</v>
+      </c>
+      <c r="AG12" s="1">
+        <f t="shared" si="5"/>
+        <v>3.2222222222222223</v>
+      </c>
+      <c r="AH12" s="1">
+        <f t="shared" si="5"/>
+        <v>-5.2110195159912012E-2</v>
+      </c>
+      <c r="AI12" s="1">
+        <f t="shared" si="5"/>
+        <v>7.5702375835842328E-2</v>
+      </c>
+      <c r="AJ12" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AK12" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -1374,7 +1703,7 @@
         <v>-0.16784495223652218</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -1429,33 +1758,33 @@
         <v>-0.17810434211384119</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <f>AVERAGE(B3:B14)</f>
         <v>0.55775104308982204</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ref="C15:H15" si="3">AVERAGE(C3:C14)</f>
+        <f t="shared" ref="C15:H15" si="6">AVERAGE(C3:C14)</f>
         <v>11.416666666666666</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>11.666666666666666</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4.333333333333333</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.32804563641548112</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-6.0833796858787488E-2</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J15" s="1">
@@ -1488,7 +1817,7 @@
         <v>1.6496443271636962</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -1879,31 +2208,31 @@
         <v>0.75720627936621465</v>
       </c>
       <c r="L28" s="1">
-        <f t="shared" ref="L28:R28" si="4">AVERAGE(L3:L26)</f>
+        <f t="shared" ref="L28:R28" si="7">AVERAGE(L3:L26)</f>
         <v>13.416666666666666</v>
       </c>
       <c r="M28" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7.833333333333333</v>
       </c>
       <c r="N28" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8.5416666666666661</v>
       </c>
       <c r="O28" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-3.4471074740091937E-2</v>
       </c>
       <c r="P28" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-0.1195586312900888</v>
       </c>
       <c r="Q28" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-1.1418809493382739E-2</v>
       </c>
       <c r="R28" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>-1.3877787807814457E-17</v>
       </c>
     </row>

</xml_diff>